<commit_message>
Project is ready to develop
</commit_message>
<xml_diff>
--- a/BICExtractor/Data/Config.xlsx
+++ b/BICExtractor/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\test-open\BICExtractor\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D816F74B-3125-41F5-8B4E-3B940A973735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -84,14 +84,7 @@
     <t>System exception.</t>
   </si>
   <si>
-    <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
     <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -122,6 +115,18 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>tempPath</t>
+  </si>
+  <si>
+    <t>outputPath</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>logF_BusinessProcessName</t>
   </si>
 </sst>
 </file>
@@ -185,7 +190,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -201,9 +206,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -241,7 +246,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -347,7 +352,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -499,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -547,25 +552,25 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1624,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1648,7 +1653,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1670,7 +1675,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1681,7 +1686,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1692,7 +1697,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2682,8 +2687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2702,7 +2707,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2730,8 +2735,22 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Now robot can send a email to admin if error happend
</commit_message>
<xml_diff>
--- a/BICExtractor/Data/Config.xlsx
+++ b/BICExtractor/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\test-open\BICExtractor\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D816F74B-3125-41F5-8B4E-3B940A973735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACAD82D-1207-4225-9BC9-25298D4FAC78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
+  </si>
+  <si>
+    <t>admEmail</t>
+  </si>
+  <si>
+    <t>server</t>
   </si>
 </sst>
 </file>
@@ -504,7 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2687,8 +2693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2751,8 +2757,22 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
add bounds of data to Config
</commit_message>
<xml_diff>
--- a/BICExtractor/Data/Config.xlsx
+++ b/BICExtractor/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\test-open\BICExtractor\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACAD82D-1207-4225-9BC9-25298D4FAC78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F70B3E3-5F62-491B-A3FB-997DBD861F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>server</t>
+  </si>
+  <si>
+    <t>beginPointer</t>
+  </si>
+  <si>
+    <t>endPointer</t>
   </si>
 </sst>
 </file>
@@ -2694,7 +2700,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2773,8 +2779,22 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>